<commit_message>
Adding files with addresses for Viz
</commit_message>
<xml_diff>
--- a/Harris_County_Schools.xlsx
+++ b/Harris_County_Schools.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8a3d0d43911148d9/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sofiwolfes/Documents/BOOTCAMP/Data_Analytics/Final_Project_MASAS/Final_Project_MASAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="128" documentId="8_{98301D0D-52C2-4BBE-A002-254D64C1528B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90D40F72-B19C-45F7-89AD-8C9A8CCEAA40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFA7504-EB14-A14F-AAC4-C1458F5BAEC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F3A26A55-937B-4EB9-86EC-48C53E16294E}"/>
+    <workbookView xWindow="840" yWindow="500" windowWidth="27420" windowHeight="17500" activeTab="1" xr2:uid="{F3A26A55-937B-4EB9-86EC-48C53E16294E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,8 +28,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="145">
   <si>
     <t>District Name</t>
   </si>
@@ -285,13 +284,199 @@
   </si>
   <si>
     <t>3 - 12</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Zip Code</t>
+  </si>
+  <si>
+    <t>2410 Hamilton St, Houston, TX 77004</t>
+  </si>
+  <si>
+    <t>6711 Bellfort Ave APT 4, Houston, TX 77087</t>
+  </si>
+  <si>
+    <t>12825 Summit Ridge Dr, Houston, TX 77085</t>
+  </si>
+  <si>
+    <t>4223-4201 J St, Houston, TX 77072</t>
+  </si>
+  <si>
+    <t>5503 El Camino Del Rey St, Houston, TX 77081</t>
+  </si>
+  <si>
+    <t>5618 11th St, Katy, TX 77493</t>
+  </si>
+  <si>
+    <t>5807 Calhoun Rd, Houston, TX 77021</t>
+  </si>
+  <si>
+    <t>9701 Almeda Genoa Rd, Houston, TX 77075</t>
+  </si>
+  <si>
+    <t>3420 Almeda Genoa Rd, Houston, TX 77047</t>
+  </si>
+  <si>
+    <t>20625 Clay Rd, Katy, TX 77449</t>
+  </si>
+  <si>
+    <t>207 Peach St, Tomball, TX 77375</t>
+  </si>
+  <si>
+    <t>3920 Stoney Brook Dr, Houston, TX 77063</t>
+  </si>
+  <si>
+    <t>6648 Hornwood Dr, Houston, TX 77074</t>
+  </si>
+  <si>
+    <t>2525 Murworth Dr #100, Houston, TX 77054</t>
+  </si>
+  <si>
+    <t>6001 Gulf Fwy, Houston, TX 77023</t>
+  </si>
+  <si>
+    <t>6403 Addicks Clodine Rd, Houston, TX 77083</t>
+  </si>
+  <si>
+    <t>7310 Bowie St, Houston, TX 77012</t>
+  </si>
+  <si>
+    <t>413 E 13th St, Houston, TX 77008</t>
+  </si>
+  <si>
+    <t>2727 Spring Creek Dr, Spring, TX 77373</t>
+  </si>
+  <si>
+    <t>13663 S Main St, Houston, TX 77035</t>
+  </si>
+  <si>
+    <t>4450 Harrisburg Blvd, Houston, TX 77011</t>
+  </si>
+  <si>
+    <t>2950 Broadway St, Houston, TX 77017</t>
+  </si>
+  <si>
+    <t>12707 Cullen Blvd, Houston, TX 77047</t>
+  </si>
+  <si>
+    <t>5610 Gulfton St, Houston, TX 77081</t>
+  </si>
+  <si>
+    <t>3333 Bering Dr, Houston, TX 77057</t>
+  </si>
+  <si>
+    <t>8282 Bissonnet St Ste. 400, Houston, TX 77074</t>
+  </si>
+  <si>
+    <t>5052 Scott St, Houston, TX 77004</t>
+  </si>
+  <si>
+    <t>11503 Martin Luther King Blvd, Houston, TX 77048</t>
+  </si>
+  <si>
+    <t>13334 Wallisville Rd, Houston, TX 77049</t>
+  </si>
+  <si>
+    <t>5025 S Willow Dr, Houston, TX 77035</t>
+  </si>
+  <si>
+    <t>12121 Veterans Memorial Dr, Houston, TX 77067</t>
+  </si>
+  <si>
+    <t>3000 Trulley St, Houston, TX 77004</t>
+  </si>
+  <si>
+    <t>6565 De Moss Dr, Houston, TX 77074</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Aldine_ISD</t>
+  </si>
+  <si>
+    <t>Alief_ISD</t>
+  </si>
+  <si>
+    <t>Aristoi_Classical_Academy</t>
+  </si>
+  <si>
+    <t>Beta_Academy</t>
+  </si>
+  <si>
+    <t>Channelview_ISD</t>
+  </si>
+  <si>
+    <t>Crosby_ISD</t>
+  </si>
+  <si>
+    <t>Cypress_Fairbanks_ISD</t>
+  </si>
+  <si>
+    <t>Deer_Park_ISD</t>
+  </si>
+  <si>
+    <t>Galena_Park_ISD</t>
+  </si>
+  <si>
+    <t>Goose_Creek_ISD</t>
+  </si>
+  <si>
+    <t>Harmony_Schools</t>
+  </si>
+  <si>
+    <t>Harmony_Schools_South</t>
+  </si>
+  <si>
+    <t>Harmony_Schools_West</t>
+  </si>
+  <si>
+    <t>Houston_ISD</t>
+  </si>
+  <si>
+    <t>Huffman_ISD</t>
+  </si>
+  <si>
+    <t>Humble_ISD</t>
+  </si>
+  <si>
+    <t>Katy_ISD</t>
+  </si>
+  <si>
+    <t>Klein_ISD</t>
+  </si>
+  <si>
+    <t>La_Porte_ISD</t>
+  </si>
+  <si>
+    <t>Pasadena_ISD</t>
+  </si>
+  <si>
+    <t>Sheldon_ISD</t>
+  </si>
+  <si>
+    <t>Spring_Branch_ISD</t>
+  </si>
+  <si>
+    <t>Spring_ISD</t>
+  </si>
+  <si>
+    <t>Tomball_ISD</t>
+  </si>
+  <si>
+    <t>Yes_Prep_Schools</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +487,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -328,12 +522,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,18 +845,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7CDBA2E-414A-46EB-851C-07ED6CA54EC0}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="40.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +870,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -689,7 +884,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -703,7 +898,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -717,7 +912,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -731,7 +926,7 @@
         <v>62000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -745,7 +940,7 @@
         <v>41724</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -759,7 +954,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -773,7 +968,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -787,7 +982,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -801,7 +996,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -815,7 +1010,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -829,7 +1024,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -843,7 +1038,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -857,7 +1052,7 @@
         <v>9572</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -871,7 +1066,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -885,7 +1080,7 @@
         <v>6319</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -899,7 +1094,7 @@
         <v>116512</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -913,7 +1108,7 @@
         <v>12287</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -927,7 +1122,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -941,7 +1136,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -955,7 +1150,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -969,7 +1164,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -983,7 +1178,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -997,7 +1192,7 @@
         <v>21918</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1011,7 +1206,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1025,7 +1220,7 @@
         <v>23318</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1039,7 +1234,7 @@
         <v>15267</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1053,7 +1248,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1067,7 +1262,7 @@
         <v>5987</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1081,7 +1276,7 @@
         <v>3677</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1095,7 +1290,7 @@
         <v>3992</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1109,7 +1304,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1123,7 +1318,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1137,7 +1332,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1151,7 +1346,7 @@
         <v>196550</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1165,7 +1360,7 @@
         <v>3439</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1179,7 +1374,7 @@
         <v>45528</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>40</v>
       </c>
@@ -1193,7 +1388,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>41</v>
       </c>
@@ -1207,7 +1402,7 @@
         <v>84176</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>42</v>
       </c>
@@ -1221,7 +1416,7 @@
         <v>52824</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>43</v>
       </c>
@@ -1235,7 +1430,7 @@
         <v>6999</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -1249,7 +1444,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>45</v>
       </c>
@@ -1263,7 +1458,7 @@
         <v>5064</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>46</v>
       </c>
@@ -1277,7 +1472,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>47</v>
       </c>
@@ -1291,7 +1486,7 @@
         <v>50614</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>48</v>
       </c>
@@ -1305,7 +1500,7 @@
         <v>1556</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>49</v>
       </c>
@@ -1319,7 +1514,7 @@
         <v>1335</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -1333,7 +1528,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>51</v>
       </c>
@@ -1347,7 +1542,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>52</v>
       </c>
@@ -1361,7 +1556,7 @@
         <v>10206</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>53</v>
       </c>
@@ -1375,7 +1570,7 @@
         <v>1703</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>54</v>
       </c>
@@ -1389,7 +1584,7 @@
         <v>33288</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -1403,7 +1598,7 @@
         <v>33567</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>56</v>
       </c>
@@ -1417,7 +1612,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>57</v>
       </c>
@@ -1431,7 +1626,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>58</v>
       </c>
@@ -1445,7 +1640,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>59</v>
       </c>
@@ -1459,7 +1654,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>60</v>
       </c>
@@ -1473,7 +1668,7 @@
         <v>1333</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>61</v>
       </c>
@@ -1487,7 +1682,7 @@
         <v>18666</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>62</v>
       </c>
@@ -1501,7 +1696,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>63</v>
       </c>
@@ -1515,7 +1710,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>64</v>
       </c>
@@ -1529,7 +1724,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>65</v>
       </c>
@@ -1547,4 +1742,1267 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5709A96E-A992-D042-A699-87DFBFFAD319}">
+  <dimension ref="A1:J63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N30" sqref="N30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <v>152</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2">
+        <v>77004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>851</v>
+      </c>
+      <c r="E3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3">
+        <v>77087</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4">
+        <v>248</v>
+      </c>
+      <c r="E4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4">
+        <v>77085</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="2">
+        <v>62000</v>
+      </c>
+      <c r="I5" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5">
+        <v>77073</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="2">
+        <v>41724</v>
+      </c>
+      <c r="I6" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6">
+        <v>77411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>331</v>
+      </c>
+      <c r="E7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F7">
+        <v>77072</v>
+      </c>
+      <c r="I7" t="s">
+        <v>122</v>
+      </c>
+      <c r="J7">
+        <v>77493</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>502</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8">
+        <v>77081</v>
+      </c>
+      <c r="I8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J8">
+        <v>77075</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1079</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9">
+        <v>77493</v>
+      </c>
+      <c r="I9" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9">
+        <v>77530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="2">
+        <v>470</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10">
+        <v>77021</v>
+      </c>
+      <c r="I10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J10">
+        <v>77532</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="2">
+        <v>751</v>
+      </c>
+      <c r="E11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F11">
+        <v>77075</v>
+      </c>
+      <c r="I11" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11">
+        <v>77065</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="2">
+        <v>93</v>
+      </c>
+      <c r="E12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
+        <v>77047</v>
+      </c>
+      <c r="I12" t="s">
+        <v>127</v>
+      </c>
+      <c r="J12">
+        <v>77536</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="2">
+        <v>300</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13">
+        <v>77449</v>
+      </c>
+      <c r="I13" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13">
+        <v>77015</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="2">
+        <v>9572</v>
+      </c>
+      <c r="I14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J14">
+        <v>77522</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="2">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15">
+        <v>77375</v>
+      </c>
+      <c r="I15" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15">
+        <v>77038</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6319</v>
+      </c>
+      <c r="I16" t="s">
+        <v>131</v>
+      </c>
+      <c r="J16">
+        <v>77099</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="2">
+        <v>116512</v>
+      </c>
+      <c r="I17" t="s">
+        <v>132</v>
+      </c>
+      <c r="J17">
+        <v>77478</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="2">
+        <v>12287</v>
+      </c>
+      <c r="I18" t="s">
+        <v>133</v>
+      </c>
+      <c r="J18">
+        <v>77092</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" s="2">
+        <v>707</v>
+      </c>
+      <c r="E19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F19">
+        <v>77063</v>
+      </c>
+      <c r="I19" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19">
+        <v>77336</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" s="2">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20">
+        <v>77004</v>
+      </c>
+      <c r="I20" t="s">
+        <v>135</v>
+      </c>
+      <c r="J20">
+        <v>77338</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2">
+        <v>846</v>
+      </c>
+      <c r="I21" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21">
+        <v>77494</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="2">
+        <v>216</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22">
+        <v>77074</v>
+      </c>
+      <c r="I22" t="s">
+        <v>137</v>
+      </c>
+      <c r="J22">
+        <v>77379</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="2">
+        <v>206</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23">
+        <v>77054</v>
+      </c>
+      <c r="I23" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23">
+        <v>77571</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="2">
+        <v>21918</v>
+      </c>
+      <c r="I24" t="s">
+        <v>139</v>
+      </c>
+      <c r="J24">
+        <v>77502</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="2">
+        <v>661</v>
+      </c>
+      <c r="E25" t="s">
+        <v>99</v>
+      </c>
+      <c r="F25">
+        <v>77023</v>
+      </c>
+      <c r="I25" t="s">
+        <v>140</v>
+      </c>
+      <c r="J25">
+        <v>77044</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="2">
+        <v>23318</v>
+      </c>
+      <c r="I26" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26">
+        <v>77024</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="2">
+        <v>15267</v>
+      </c>
+      <c r="I27" t="s">
+        <v>142</v>
+      </c>
+      <c r="J27">
+        <v>77090</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" s="2">
+        <v>714</v>
+      </c>
+      <c r="I28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J28">
+        <v>77375</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5987</v>
+      </c>
+      <c r="I29" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29">
+        <v>77074</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" s="2">
+        <v>3677</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="2">
+        <v>3992</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" s="2">
+        <v>131</v>
+      </c>
+      <c r="E32" t="s">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>77083</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="2">
+        <v>648</v>
+      </c>
+      <c r="E33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F33">
+        <v>77012</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="2">
+        <v>178</v>
+      </c>
+      <c r="E34" t="s">
+        <v>102</v>
+      </c>
+      <c r="F34">
+        <v>77008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D35" s="2">
+        <v>196550</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D36" s="2">
+        <v>3439</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D37" s="2">
+        <v>45528</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D38" s="2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D39" s="2">
+        <v>84176</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="2">
+        <v>52824</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D41" s="2">
+        <v>6999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" t="s">
+        <v>2</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2">
+        <v>392</v>
+      </c>
+      <c r="E42" t="s">
+        <v>103</v>
+      </c>
+      <c r="F42">
+        <v>77373</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D43" s="2">
+        <v>5064</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="2">
+        <v>260</v>
+      </c>
+      <c r="E44" t="s">
+        <v>104</v>
+      </c>
+      <c r="F44">
+        <v>77035</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="2">
+        <v>50614</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="2">
+        <v>1556</v>
+      </c>
+      <c r="E46" t="s">
+        <v>105</v>
+      </c>
+      <c r="F46">
+        <v>77011</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" t="s">
+        <v>2</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="2">
+        <v>1335</v>
+      </c>
+      <c r="E47" t="s">
+        <v>106</v>
+      </c>
+      <c r="F47">
+        <v>77017</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D48" s="2">
+        <v>120</v>
+      </c>
+      <c r="E48" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48">
+        <v>77047</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>2</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="2">
+        <v>1095</v>
+      </c>
+      <c r="E49" t="s">
+        <v>108</v>
+      </c>
+      <c r="F49">
+        <v>77081</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" s="2">
+        <v>10206</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" t="s">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D51" s="2">
+        <v>1703</v>
+      </c>
+      <c r="E51" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51">
+        <v>77057</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D52" s="2">
+        <v>33288</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="2">
+        <v>33567</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="2">
+        <v>497</v>
+      </c>
+      <c r="E54" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54">
+        <v>77074</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="2">
+        <v>182</v>
+      </c>
+      <c r="E55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55">
+        <v>77004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D56" s="2">
+        <v>432</v>
+      </c>
+      <c r="E56" t="s">
+        <v>112</v>
+      </c>
+      <c r="F56">
+        <v>77048</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D57" s="2">
+        <v>718</v>
+      </c>
+      <c r="E57" t="s">
+        <v>113</v>
+      </c>
+      <c r="F57">
+        <v>77049</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" t="s">
+        <v>2</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="2">
+        <v>1333</v>
+      </c>
+      <c r="E58" t="s">
+        <v>114</v>
+      </c>
+      <c r="F58">
+        <v>77035</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>61</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D59" s="2">
+        <v>18666</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>62</v>
+      </c>
+      <c r="B60" t="s">
+        <v>2</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="2">
+        <v>440</v>
+      </c>
+      <c r="E60" t="s">
+        <v>115</v>
+      </c>
+      <c r="F60">
+        <v>77067</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>63</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D61" s="2">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="2">
+        <v>221</v>
+      </c>
+      <c r="E62" t="s">
+        <v>116</v>
+      </c>
+      <c r="F62">
+        <v>77004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63" t="s">
+        <v>2</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" s="2">
+        <v>13455</v>
+      </c>
+      <c r="E63" t="s">
+        <v>117</v>
+      </c>
+      <c r="F63">
+        <v>77074</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>